<commit_message>
Update DR# 605 BDO UNIBANK GEMALTO(VIRTUALCARDS_VISA_MC)_09_24_2020.xlsx
</commit_message>
<xml_diff>
--- a/DR# 605 BDO UNIBANK GEMALTO(VIRTUALCARDS_VISA_MC)_09_24_2020.xlsx
+++ b/DR# 605 BDO UNIBANK GEMALTO(VIRTUALCARDS_VISA_MC)_09_24_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11BED9DD-8321-4D55-859D-5BA7F6DE1947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5230CBA-B4FB-41C7-AABC-AB5957F43D6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>DELIVERY RECEIPT</t>
   </si>
@@ -161,9 +161,6 @@
     <t>TO: BDO UNIBANK</t>
   </si>
   <si>
-    <t>Address: GEMALTO LAGUNA</t>
-  </si>
-  <si>
     <t>BDO VIRTUAL CARD VISA CLASSIC/ELITE</t>
   </si>
   <si>
@@ -171,6 +168,12 @@
   </si>
   <si>
     <t>09/24/2020</t>
+  </si>
+  <si>
+    <t>Address: GEMALTO PH, BLDG. 7A SOUTHERN LUZON INDUSTRIAL COMPLEX</t>
+  </si>
+  <si>
+    <t>BATINO CALAMBA CITY, LAGUNA 4027, PHILIPPINES</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -488,6 +491,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -497,15 +509,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,13 +968,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1186,13 +1190,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1379,7 +1383,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1407,13 +1411,13 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="50.25" customHeight="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1450,24 +1454,26 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1">
-      <c r="A11" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
+      <c r="A11" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
     </row>
     <row r="12" spans="1:13" ht="18">
-      <c r="A12" s="23"/>
+      <c r="A12" s="50" t="s">
+        <v>30</v>
+      </c>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="23"/>
@@ -1503,7 +1509,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="36">
         <v>5200</v>
@@ -1512,15 +1518,15 @@
         <v>5200</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="36">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="49" t="s">
-        <v>28</v>
+      <c r="B16" s="46" t="s">
+        <v>27</v>
       </c>
       <c r="C16" s="29">
         <v>12200</v>
@@ -1528,8 +1534,8 @@
       <c r="D16" s="29">
         <v>12200</v>
       </c>
-      <c r="E16" s="48" t="s">
-        <v>29</v>
+      <c r="E16" s="45" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18">

</xml_diff>